<commit_message>
Add battery status setpoints
</commit_message>
<xml_diff>
--- a/hello_world.xlsx
+++ b/hello_world.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AQ2"/>
+  <dimension ref="A1:AW2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -638,6 +638,36 @@
           <t>SW_Check</t>
         </is>
       </c>
+      <c r="AR1" t="inlineStr">
+        <is>
+          <t>CellTempMin</t>
+        </is>
+      </c>
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>CellTempMax</t>
+        </is>
+      </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>CellTempRange</t>
+        </is>
+      </c>
+      <c r="AU1" t="inlineStr">
+        <is>
+          <t>CellVoltageMin</t>
+        </is>
+      </c>
+      <c r="AV1" t="inlineStr">
+        <is>
+          <t>CellVoltageMax</t>
+        </is>
+      </c>
+      <c r="AW1" t="inlineStr">
+        <is>
+          <t>CellVoltageRange</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -853,6 +883,36 @@
       <c r="AQ2" t="inlineStr">
         <is>
           <t>"IO"</t>
+        </is>
+      </c>
+      <c r="AR2" t="inlineStr">
+        <is>
+          <t>5.00</t>
+        </is>
+      </c>
+      <c r="AS2" t="inlineStr">
+        <is>
+          <t>40.00</t>
+        </is>
+      </c>
+      <c r="AT2" t="inlineStr">
+        <is>
+          <t>15.00</t>
+        </is>
+      </c>
+      <c r="AU2" t="inlineStr">
+        <is>
+          <t>2.50</t>
+        </is>
+      </c>
+      <c r="AV2" t="inlineStr">
+        <is>
+          <t>4.20</t>
+        </is>
+      </c>
+      <c r="AW2" t="inlineStr">
+        <is>
+          <t>50.00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Flash SW (BMCe and CMC)
</commit_message>
<xml_diff>
--- a/hello_world.xlsx
+++ b/hello_world.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:GD2"/>
+  <dimension ref="A1:GH2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,880 +475,900 @@
       </c>
       <c r="K1" t="inlineStr">
         <is>
+          <t>BCMe Flash SW</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>CMC1 Flash SW</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>CMC2 Flash SW</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>CMC3 Flash SW</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
           <t>BCMe Begin BL</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>CMC1 Begin BL</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>CMC2 Begin BL</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>CMC3 Begin BL</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>BatConfigPSet</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>VehiclePSet</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>TargetMarket</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>ConfigNamePSet</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>ThermoPSet</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>NameVehiclePSet</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>NameTargetMarket</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>CMC1 HW</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>CMC2 HW</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>CMC3 HW</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>CMC1 Serial</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>CMC2 Serial</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>CMC3 Serial</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>BCMe HW</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>BCMe HW Serial</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>BCMe SW Serial</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>CMC1 HW Serial</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>CMC2 HW Serial</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>CMC3 HW Serial</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>CMC1 SW Serial</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>CMC2 SW Serial</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>CMC3 SW Serial</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>preFlashBCMeSW_Check</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>PostFlashBCMeSW_Check</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>dataSet_download_Check</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>PostDSDL_BCMeSW_Check</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>preFlashCMCSW_Check</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>PostFlashCMCSW_Check</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>SW_Check</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>CellTempMin</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="AW1" t="inlineStr">
         <is>
           <t>CellTempMax</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
+      <c r="AX1" t="inlineStr">
         <is>
           <t>CellTempRange</t>
         </is>
       </c>
-      <c r="AU1" t="inlineStr">
+      <c r="AY1" t="inlineStr">
         <is>
           <t>CellVoltageMin</t>
         </is>
       </c>
-      <c r="AV1" t="inlineStr">
+      <c r="AZ1" t="inlineStr">
         <is>
           <t>CellVoltageMax</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="BA1" t="inlineStr">
         <is>
           <t>CellVoltageRange</t>
         </is>
       </c>
-      <c r="AX1" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>CellTempCheck</t>
         </is>
       </c>
-      <c r="AY1" t="inlineStr">
+      <c r="BC1" t="inlineStr">
         <is>
           <t>CellTemp1</t>
         </is>
       </c>
-      <c r="AZ1" t="inlineStr">
+      <c r="BD1" t="inlineStr">
         <is>
           <t>CellTemp2</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="BE1" t="inlineStr">
         <is>
           <t>CellTemp3</t>
         </is>
       </c>
-      <c r="BB1" t="inlineStr">
+      <c r="BF1" t="inlineStr">
         <is>
           <t>CellTemp4</t>
         </is>
       </c>
-      <c r="BC1" t="inlineStr">
+      <c r="BG1" t="inlineStr">
         <is>
           <t>CellTemp5</t>
         </is>
       </c>
-      <c r="BD1" t="inlineStr">
+      <c r="BH1" t="inlineStr">
         <is>
           <t>CellTemp6</t>
         </is>
       </c>
-      <c r="BE1" t="inlineStr">
+      <c r="BI1" t="inlineStr">
         <is>
           <t>CellTemp7</t>
         </is>
       </c>
-      <c r="BF1" t="inlineStr">
+      <c r="BJ1" t="inlineStr">
         <is>
           <t>CellTemp8</t>
         </is>
       </c>
-      <c r="BG1" t="inlineStr">
+      <c r="BK1" t="inlineStr">
         <is>
           <t>CellTemp9</t>
         </is>
       </c>
-      <c r="BH1" t="inlineStr">
+      <c r="BL1" t="inlineStr">
         <is>
           <t>CellTemp10</t>
         </is>
       </c>
-      <c r="BI1" t="inlineStr">
+      <c r="BM1" t="inlineStr">
         <is>
           <t>CellTemp11</t>
         </is>
       </c>
-      <c r="BJ1" t="inlineStr">
+      <c r="BN1" t="inlineStr">
         <is>
           <t>CellTemp12</t>
         </is>
       </c>
-      <c r="BK1" t="inlineStr">
+      <c r="BO1" t="inlineStr">
         <is>
           <t>CellTemp13</t>
         </is>
       </c>
-      <c r="BL1" t="inlineStr">
+      <c r="BP1" t="inlineStr">
         <is>
           <t>CellTemp14</t>
         </is>
       </c>
-      <c r="BM1" t="inlineStr">
+      <c r="BQ1" t="inlineStr">
         <is>
           <t>CellTemp15</t>
         </is>
       </c>
-      <c r="BN1" t="inlineStr">
+      <c r="BR1" t="inlineStr">
         <is>
           <t>CellTemp16</t>
         </is>
       </c>
-      <c r="BO1" t="inlineStr">
+      <c r="BS1" t="inlineStr">
         <is>
           <t>CellTemp17</t>
         </is>
       </c>
-      <c r="BP1" t="inlineStr">
+      <c r="BT1" t="inlineStr">
         <is>
           <t>CellTemp18</t>
         </is>
       </c>
-      <c r="BQ1" t="inlineStr">
+      <c r="BU1" t="inlineStr">
         <is>
           <t>CellTemp19</t>
         </is>
       </c>
-      <c r="BR1" t="inlineStr">
+      <c r="BV1" t="inlineStr">
         <is>
           <t>CellTemp20</t>
         </is>
       </c>
-      <c r="BS1" t="inlineStr">
+      <c r="BW1" t="inlineStr">
         <is>
           <t>CellTemp21</t>
         </is>
       </c>
-      <c r="BT1" t="inlineStr">
+      <c r="BX1" t="inlineStr">
         <is>
           <t>CellTemp22</t>
         </is>
       </c>
-      <c r="BU1" t="inlineStr">
+      <c r="BY1" t="inlineStr">
         <is>
           <t>CellTemp23</t>
         </is>
       </c>
-      <c r="BV1" t="inlineStr">
+      <c r="BZ1" t="inlineStr">
         <is>
           <t>CellTemp24</t>
         </is>
       </c>
-      <c r="BW1" t="inlineStr">
+      <c r="CA1" t="inlineStr">
         <is>
           <t>CellTempRange</t>
         </is>
       </c>
-      <c r="BX1" t="inlineStr">
+      <c r="CB1" t="inlineStr">
         <is>
           <t>CellVolt1</t>
         </is>
       </c>
-      <c r="BY1" t="inlineStr">
+      <c r="CC1" t="inlineStr">
         <is>
           <t>CellVolt2</t>
         </is>
       </c>
-      <c r="BZ1" t="inlineStr">
+      <c r="CD1" t="inlineStr">
         <is>
           <t>CellVolt3</t>
         </is>
       </c>
-      <c r="CA1" t="inlineStr">
+      <c r="CE1" t="inlineStr">
         <is>
           <t>CellVolt4</t>
         </is>
       </c>
-      <c r="CB1" t="inlineStr">
+      <c r="CF1" t="inlineStr">
         <is>
           <t>CellVolt5</t>
         </is>
       </c>
-      <c r="CC1" t="inlineStr">
+      <c r="CG1" t="inlineStr">
         <is>
           <t>CellVolt6</t>
         </is>
       </c>
-      <c r="CD1" t="inlineStr">
+      <c r="CH1" t="inlineStr">
         <is>
           <t>CellVolt7</t>
         </is>
       </c>
-      <c r="CE1" t="inlineStr">
+      <c r="CI1" t="inlineStr">
         <is>
           <t>CellVolt8</t>
         </is>
       </c>
-      <c r="CF1" t="inlineStr">
+      <c r="CJ1" t="inlineStr">
         <is>
           <t>CellVolt9</t>
         </is>
       </c>
-      <c r="CG1" t="inlineStr">
+      <c r="CK1" t="inlineStr">
         <is>
           <t>CellVolt10</t>
         </is>
       </c>
-      <c r="CH1" t="inlineStr">
+      <c r="CL1" t="inlineStr">
         <is>
           <t>CellVolt11</t>
         </is>
       </c>
-      <c r="CI1" t="inlineStr">
+      <c r="CM1" t="inlineStr">
         <is>
           <t>CellVolt12</t>
         </is>
       </c>
-      <c r="CJ1" t="inlineStr">
+      <c r="CN1" t="inlineStr">
         <is>
           <t>CellVolt13</t>
         </is>
       </c>
-      <c r="CK1" t="inlineStr">
+      <c r="CO1" t="inlineStr">
         <is>
           <t>CellVolt14</t>
         </is>
       </c>
-      <c r="CL1" t="inlineStr">
+      <c r="CP1" t="inlineStr">
         <is>
           <t>CellVolt15</t>
         </is>
       </c>
-      <c r="CM1" t="inlineStr">
+      <c r="CQ1" t="inlineStr">
         <is>
           <t>CellVolt16</t>
         </is>
       </c>
-      <c r="CN1" t="inlineStr">
+      <c r="CR1" t="inlineStr">
         <is>
           <t>CellVolt17</t>
         </is>
       </c>
-      <c r="CO1" t="inlineStr">
+      <c r="CS1" t="inlineStr">
         <is>
           <t>CellVolt18</t>
         </is>
       </c>
-      <c r="CP1" t="inlineStr">
+      <c r="CT1" t="inlineStr">
         <is>
           <t>CellVolt19</t>
         </is>
       </c>
-      <c r="CQ1" t="inlineStr">
+      <c r="CU1" t="inlineStr">
         <is>
           <t>CellVolt20</t>
         </is>
       </c>
-      <c r="CR1" t="inlineStr">
+      <c r="CV1" t="inlineStr">
         <is>
           <t>CellVolt21</t>
         </is>
       </c>
-      <c r="CS1" t="inlineStr">
+      <c r="CW1" t="inlineStr">
         <is>
           <t>CellVolt22</t>
         </is>
       </c>
-      <c r="CT1" t="inlineStr">
+      <c r="CX1" t="inlineStr">
         <is>
           <t>CellVolt23</t>
         </is>
       </c>
-      <c r="CU1" t="inlineStr">
+      <c r="CY1" t="inlineStr">
         <is>
           <t>CellVolt24</t>
         </is>
       </c>
-      <c r="CV1" t="inlineStr">
+      <c r="CZ1" t="inlineStr">
         <is>
           <t>CellVolt25</t>
         </is>
       </c>
-      <c r="CW1" t="inlineStr">
+      <c r="DA1" t="inlineStr">
         <is>
           <t>CellVolt26</t>
         </is>
       </c>
-      <c r="CX1" t="inlineStr">
+      <c r="DB1" t="inlineStr">
         <is>
           <t>CellVolt27</t>
         </is>
       </c>
-      <c r="CY1" t="inlineStr">
+      <c r="DC1" t="inlineStr">
         <is>
           <t>CellVolt28</t>
         </is>
       </c>
-      <c r="CZ1" t="inlineStr">
+      <c r="DD1" t="inlineStr">
         <is>
           <t>CellVolt29</t>
         </is>
       </c>
-      <c r="DA1" t="inlineStr">
+      <c r="DE1" t="inlineStr">
         <is>
           <t>CellVolt30</t>
         </is>
       </c>
-      <c r="DB1" t="inlineStr">
+      <c r="DF1" t="inlineStr">
         <is>
           <t>CellVolt31</t>
         </is>
       </c>
-      <c r="DC1" t="inlineStr">
+      <c r="DG1" t="inlineStr">
         <is>
           <t>CellVolt32</t>
         </is>
       </c>
-      <c r="DD1" t="inlineStr">
+      <c r="DH1" t="inlineStr">
         <is>
           <t>CellVolt33</t>
         </is>
       </c>
-      <c r="DE1" t="inlineStr">
+      <c r="DI1" t="inlineStr">
         <is>
           <t>CellVolt34</t>
         </is>
       </c>
-      <c r="DF1" t="inlineStr">
+      <c r="DJ1" t="inlineStr">
         <is>
           <t>CellVolt35</t>
         </is>
       </c>
-      <c r="DG1" t="inlineStr">
+      <c r="DK1" t="inlineStr">
         <is>
           <t>CellVolt36</t>
         </is>
       </c>
-      <c r="DH1" t="inlineStr">
+      <c r="DL1" t="inlineStr">
         <is>
           <t>CellVolt37</t>
         </is>
       </c>
-      <c r="DI1" t="inlineStr">
+      <c r="DM1" t="inlineStr">
         <is>
           <t>CellVolt38</t>
         </is>
       </c>
-      <c r="DJ1" t="inlineStr">
+      <c r="DN1" t="inlineStr">
         <is>
           <t>CellVolt39</t>
         </is>
       </c>
-      <c r="DK1" t="inlineStr">
+      <c r="DO1" t="inlineStr">
         <is>
           <t>CellVolt40</t>
         </is>
       </c>
-      <c r="DL1" t="inlineStr">
+      <c r="DP1" t="inlineStr">
         <is>
           <t>CellVolt41</t>
         </is>
       </c>
-      <c r="DM1" t="inlineStr">
+      <c r="DQ1" t="inlineStr">
         <is>
           <t>CellVolt42</t>
         </is>
       </c>
-      <c r="DN1" t="inlineStr">
+      <c r="DR1" t="inlineStr">
         <is>
           <t>CellVolt43</t>
         </is>
       </c>
-      <c r="DO1" t="inlineStr">
+      <c r="DS1" t="inlineStr">
         <is>
           <t>CellVolt44</t>
         </is>
       </c>
-      <c r="DP1" t="inlineStr">
+      <c r="DT1" t="inlineStr">
         <is>
           <t>CellVolt45</t>
         </is>
       </c>
-      <c r="DQ1" t="inlineStr">
+      <c r="DU1" t="inlineStr">
         <is>
           <t>CellVolt46</t>
         </is>
       </c>
-      <c r="DR1" t="inlineStr">
+      <c r="DV1" t="inlineStr">
         <is>
           <t>CellVolt47</t>
         </is>
       </c>
-      <c r="DS1" t="inlineStr">
+      <c r="DW1" t="inlineStr">
         <is>
           <t>CellVolt48</t>
         </is>
       </c>
-      <c r="DT1" t="inlineStr">
+      <c r="DX1" t="inlineStr">
         <is>
           <t>CellVolt49</t>
         </is>
       </c>
-      <c r="DU1" t="inlineStr">
+      <c r="DY1" t="inlineStr">
         <is>
           <t>CellVolt50</t>
         </is>
       </c>
-      <c r="DV1" t="inlineStr">
+      <c r="DZ1" t="inlineStr">
         <is>
           <t>CellVolt51</t>
         </is>
       </c>
-      <c r="DW1" t="inlineStr">
+      <c r="EA1" t="inlineStr">
         <is>
           <t>CellVolt52</t>
         </is>
       </c>
-      <c r="DX1" t="inlineStr">
+      <c r="EB1" t="inlineStr">
         <is>
           <t>CellVolt53</t>
         </is>
       </c>
-      <c r="DY1" t="inlineStr">
+      <c r="EC1" t="inlineStr">
         <is>
           <t>CellVolt54</t>
         </is>
       </c>
-      <c r="DZ1" t="inlineStr">
+      <c r="ED1" t="inlineStr">
         <is>
           <t>CellVolt55</t>
         </is>
       </c>
-      <c r="EA1" t="inlineStr">
+      <c r="EE1" t="inlineStr">
         <is>
           <t>CellVolt56</t>
         </is>
       </c>
-      <c r="EB1" t="inlineStr">
+      <c r="EF1" t="inlineStr">
         <is>
           <t>CellVolt57</t>
         </is>
       </c>
-      <c r="EC1" t="inlineStr">
+      <c r="EG1" t="inlineStr">
         <is>
           <t>CellVolt58</t>
         </is>
       </c>
-      <c r="ED1" t="inlineStr">
+      <c r="EH1" t="inlineStr">
         <is>
           <t>CellVolt59</t>
         </is>
       </c>
-      <c r="EE1" t="inlineStr">
+      <c r="EI1" t="inlineStr">
         <is>
           <t>CellVolt60</t>
         </is>
       </c>
-      <c r="EF1" t="inlineStr">
+      <c r="EJ1" t="inlineStr">
         <is>
           <t>CellVolt61</t>
         </is>
       </c>
-      <c r="EG1" t="inlineStr">
+      <c r="EK1" t="inlineStr">
         <is>
           <t>CellVolt62</t>
         </is>
       </c>
-      <c r="EH1" t="inlineStr">
+      <c r="EL1" t="inlineStr">
         <is>
           <t>CellVolt63</t>
         </is>
       </c>
-      <c r="EI1" t="inlineStr">
+      <c r="EM1" t="inlineStr">
         <is>
           <t>CellVolt64</t>
         </is>
       </c>
-      <c r="EJ1" t="inlineStr">
+      <c r="EN1" t="inlineStr">
         <is>
           <t>CellVolt65</t>
         </is>
       </c>
-      <c r="EK1" t="inlineStr">
+      <c r="EO1" t="inlineStr">
         <is>
           <t>CellVolt66</t>
         </is>
       </c>
-      <c r="EL1" t="inlineStr">
+      <c r="EP1" t="inlineStr">
         <is>
           <t>CellVolt67</t>
         </is>
       </c>
-      <c r="EM1" t="inlineStr">
+      <c r="EQ1" t="inlineStr">
         <is>
           <t>CellVolt68</t>
         </is>
       </c>
-      <c r="EN1" t="inlineStr">
+      <c r="ER1" t="inlineStr">
         <is>
           <t>CellVolt69</t>
         </is>
       </c>
-      <c r="EO1" t="inlineStr">
+      <c r="ES1" t="inlineStr">
         <is>
           <t>CellVolt70</t>
         </is>
       </c>
-      <c r="EP1" t="inlineStr">
+      <c r="ET1" t="inlineStr">
         <is>
           <t>CellVolt71</t>
         </is>
       </c>
-      <c r="EQ1" t="inlineStr">
+      <c r="EU1" t="inlineStr">
         <is>
           <t>CellVolt72</t>
         </is>
       </c>
-      <c r="ER1" t="inlineStr">
+      <c r="EV1" t="inlineStr">
         <is>
           <t>CellVolt73</t>
         </is>
       </c>
-      <c r="ES1" t="inlineStr">
+      <c r="EW1" t="inlineStr">
         <is>
           <t>CellVolt74</t>
         </is>
       </c>
-      <c r="ET1" t="inlineStr">
+      <c r="EX1" t="inlineStr">
         <is>
           <t>CellVolt75</t>
         </is>
       </c>
-      <c r="EU1" t="inlineStr">
+      <c r="EY1" t="inlineStr">
         <is>
           <t>CellVolt76</t>
         </is>
       </c>
-      <c r="EV1" t="inlineStr">
+      <c r="EZ1" t="inlineStr">
         <is>
           <t>CellVolt77</t>
         </is>
       </c>
-      <c r="EW1" t="inlineStr">
+      <c r="FA1" t="inlineStr">
         <is>
           <t>CellVolt78</t>
         </is>
       </c>
-      <c r="EX1" t="inlineStr">
+      <c r="FB1" t="inlineStr">
         <is>
           <t>CellVolt79</t>
         </is>
       </c>
-      <c r="EY1" t="inlineStr">
+      <c r="FC1" t="inlineStr">
         <is>
           <t>CellVolt80</t>
         </is>
       </c>
-      <c r="EZ1" t="inlineStr">
+      <c r="FD1" t="inlineStr">
         <is>
           <t>CellVolt81</t>
         </is>
       </c>
-      <c r="FA1" t="inlineStr">
+      <c r="FE1" t="inlineStr">
         <is>
           <t>CellVolt82</t>
         </is>
       </c>
-      <c r="FB1" t="inlineStr">
+      <c r="FF1" t="inlineStr">
         <is>
           <t>CellVolt83</t>
         </is>
       </c>
-      <c r="FC1" t="inlineStr">
+      <c r="FG1" t="inlineStr">
         <is>
           <t>CellVolt84</t>
         </is>
       </c>
-      <c r="FD1" t="inlineStr">
+      <c r="FH1" t="inlineStr">
         <is>
           <t>CellVolt85</t>
         </is>
       </c>
-      <c r="FE1" t="inlineStr">
+      <c r="FI1" t="inlineStr">
         <is>
           <t>CellVolt86</t>
         </is>
       </c>
-      <c r="FF1" t="inlineStr">
+      <c r="FJ1" t="inlineStr">
         <is>
           <t>CellVolt87</t>
         </is>
       </c>
-      <c r="FG1" t="inlineStr">
+      <c r="FK1" t="inlineStr">
         <is>
           <t>CellVolt88</t>
         </is>
       </c>
-      <c r="FH1" t="inlineStr">
+      <c r="FL1" t="inlineStr">
         <is>
           <t>CellVolt89</t>
         </is>
       </c>
-      <c r="FI1" t="inlineStr">
+      <c r="FM1" t="inlineStr">
         <is>
           <t>CellVolt90</t>
         </is>
       </c>
-      <c r="FJ1" t="inlineStr">
+      <c r="FN1" t="inlineStr">
         <is>
           <t>CellVolt91</t>
         </is>
       </c>
-      <c r="FK1" t="inlineStr">
+      <c r="FO1" t="inlineStr">
         <is>
           <t>CellVolt92</t>
         </is>
       </c>
-      <c r="FL1" t="inlineStr">
+      <c r="FP1" t="inlineStr">
         <is>
           <t>CellVolt93</t>
         </is>
       </c>
-      <c r="FM1" t="inlineStr">
+      <c r="FQ1" t="inlineStr">
         <is>
           <t>CellVolt94</t>
         </is>
       </c>
-      <c r="FN1" t="inlineStr">
+      <c r="FR1" t="inlineStr">
         <is>
           <t>CellVolt95</t>
         </is>
       </c>
-      <c r="FO1" t="inlineStr">
+      <c r="FS1" t="inlineStr">
         <is>
           <t>CellVolt96</t>
         </is>
       </c>
-      <c r="FP1" t="inlineStr">
+      <c r="FT1" t="inlineStr">
         <is>
           <t>CellVoltRange</t>
         </is>
       </c>
-      <c r="FQ1" t="inlineStr">
+      <c r="FU1" t="inlineStr">
         <is>
           <t>CV_DTC1</t>
         </is>
       </c>
-      <c r="FR1" t="inlineStr">
+      <c r="FV1" t="inlineStr">
         <is>
           <t>CV_DTC2</t>
         </is>
       </c>
-      <c r="FS1" t="inlineStr">
+      <c r="FW1" t="inlineStr">
         <is>
           <t>CV_DTC3</t>
         </is>
       </c>
-      <c r="FT1" t="inlineStr">
+      <c r="FX1" t="inlineStr">
         <is>
           <t>CV_DTC4</t>
         </is>
       </c>
-      <c r="FU1" t="inlineStr">
+      <c r="FY1" t="inlineStr">
         <is>
           <t>CellVoltageMinActual</t>
         </is>
       </c>
-      <c r="FV1" t="inlineStr">
+      <c r="FZ1" t="inlineStr">
         <is>
           <t>CellVoltageMaxActual</t>
         </is>
       </c>
-      <c r="FW1" t="inlineStr">
+      <c r="GA1" t="inlineStr">
         <is>
           <t>CellTempMinActual</t>
         </is>
       </c>
-      <c r="FX1" t="inlineStr">
+      <c r="GB1" t="inlineStr">
         <is>
           <t>CellVoltageMaxActual</t>
         </is>
       </c>
-      <c r="FY1" t="inlineStr">
+      <c r="GC1" t="inlineStr">
         <is>
           <t>TempVoltageResult</t>
         </is>
       </c>
-      <c r="FZ1" t="inlineStr">
+      <c r="GD1" t="inlineStr">
         <is>
           <t>PyroCheckCount</t>
         </is>
       </c>
-      <c r="GA1" t="inlineStr">
+      <c r="GE1" t="inlineStr">
         <is>
           <t>PyroMinSet</t>
         </is>
       </c>
-      <c r="GB1" t="inlineStr">
+      <c r="GF1" t="inlineStr">
         <is>
           <t>PyroMaxSet</t>
         </is>
       </c>
-      <c r="GC1" t="inlineStr">
+      <c r="GG1" t="inlineStr">
         <is>
           <t>PyroCheckResult</t>
         </is>
       </c>
-      <c r="GD1" t="inlineStr">
+      <c r="GH1" t="inlineStr">
         <is>
           <t>PyroCheckStatus</t>
         </is>
@@ -1407,374 +1427,374 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
           <t>5022</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="P2" t="inlineStr">
         <is>
           <t>1525</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="Q2" t="inlineStr">
         <is>
           <t>1525</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="R2" t="inlineStr">
         <is>
           <t>1525</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="S2" t="inlineStr">
         <is>
           <t>0107</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
+      <c r="T2" t="inlineStr">
         <is>
           <t>0896</t>
         </is>
       </c>
-      <c r="Q2" t="inlineStr">
+      <c r="U2" t="inlineStr">
         <is>
           <t>0107</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr">
+      <c r="V2" t="inlineStr">
         <is>
           <t>82K096S3PSK0</t>
         </is>
       </c>
-      <c r="S2" t="inlineStr">
+      <c r="W2" t="inlineStr">
         <is>
           <t>DEFAULTTHERM</t>
         </is>
       </c>
-      <c r="T2" t="inlineStr">
+      <c r="X2" t="inlineStr">
         <is>
           <t>SK07809603KA</t>
         </is>
       </c>
-      <c r="U2" t="inlineStr">
+      <c r="Y2" t="inlineStr">
         <is>
           <t>DEFAULTYYYYY</t>
         </is>
       </c>
-      <c r="V2" t="inlineStr">
+      <c r="Z2" t="inlineStr">
         <is>
           <t>005</t>
         </is>
       </c>
-      <c r="W2" t="inlineStr">
+      <c r="AA2" t="inlineStr">
         <is>
           <t>005</t>
         </is>
       </c>
-      <c r="X2" t="inlineStr">
+      <c r="AB2" t="inlineStr">
         <is>
           <t>005</t>
         </is>
       </c>
-      <c r="Y2" t="inlineStr">
+      <c r="AC2" t="inlineStr">
         <is>
           <t>00000027042102910102</t>
         </is>
       </c>
-      <c r="Z2" t="inlineStr">
+      <c r="AD2" t="inlineStr">
         <is>
           <t>00000026042102910156</t>
         </is>
       </c>
-      <c r="AA2" t="inlineStr">
+      <c r="AE2" t="inlineStr">
         <is>
           <t>00000008042102910235</t>
         </is>
       </c>
-      <c r="AB2" t="inlineStr">
+      <c r="AF2" t="inlineStr">
         <is>
           <t>010</t>
         </is>
       </c>
-      <c r="AC2" t="inlineStr">
+      <c r="AG2" t="inlineStr">
         <is>
           <t>0Z1915184D</t>
         </is>
       </c>
-      <c r="AD2" t="inlineStr">
+      <c r="AH2" t="inlineStr">
         <is>
           <t>0Z1915184G</t>
         </is>
       </c>
-      <c r="AE2" t="inlineStr">
+      <c r="AI2" t="inlineStr">
         <is>
           <t>0Z1915140D</t>
         </is>
       </c>
-      <c r="AF2" t="inlineStr">
+      <c r="AJ2" t="inlineStr">
         <is>
           <t>0Z1915140D</t>
         </is>
       </c>
-      <c r="AG2" t="inlineStr">
+      <c r="AK2" t="inlineStr">
         <is>
           <t>0Z1915140D</t>
         </is>
       </c>
-      <c r="AH2" t="inlineStr">
+      <c r="AL2" t="inlineStr">
         <is>
           <t>0Z1915140F</t>
         </is>
       </c>
-      <c r="AI2" t="inlineStr">
+      <c r="AM2" t="inlineStr">
         <is>
           <t>0Z1915140F</t>
         </is>
       </c>
-      <c r="AJ2" t="inlineStr">
+      <c r="AN2" t="inlineStr">
         <is>
           <t>0Z1915140F</t>
         </is>
       </c>
-      <c r="AK2" t="inlineStr">
+      <c r="AO2" t="inlineStr">
         <is>
           <t>true</t>
         </is>
       </c>
-      <c r="AL2" t="inlineStr">
+      <c r="AP2" t="inlineStr">
         <is>
           <t>true</t>
         </is>
       </c>
-      <c r="AM2" t="inlineStr">
+      <c r="AQ2" t="inlineStr">
         <is>
           <t>true</t>
         </is>
       </c>
-      <c r="AN2" t="inlineStr">
+      <c r="AR2" t="inlineStr">
         <is>
           <t>true</t>
         </is>
       </c>
-      <c r="AO2" t="inlineStr">
+      <c r="AS2" t="inlineStr">
         <is>
           <t>true</t>
         </is>
       </c>
-      <c r="AP2" t="inlineStr">
+      <c r="AT2" t="inlineStr">
         <is>
           <t>true</t>
         </is>
       </c>
-      <c r="AQ2" t="inlineStr">
+      <c r="AU2" t="inlineStr">
         <is>
           <t>"IO"</t>
         </is>
       </c>
-      <c r="AR2" t="inlineStr">
+      <c r="AV2" t="inlineStr">
         <is>
           <t>5.00</t>
         </is>
       </c>
-      <c r="AS2" t="inlineStr">
+      <c r="AW2" t="inlineStr">
         <is>
           <t>40.00</t>
         </is>
       </c>
-      <c r="AT2" t="inlineStr">
+      <c r="AX2" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="AU2" t="inlineStr">
+      <c r="AY2" t="inlineStr">
         <is>
           <t>2.50</t>
         </is>
       </c>
-      <c r="AV2" t="inlineStr">
+      <c r="AZ2" t="inlineStr">
         <is>
           <t>4.20</t>
         </is>
       </c>
-      <c r="AW2" t="inlineStr">
+      <c r="BA2" t="inlineStr">
         <is>
           <t>50.00</t>
         </is>
       </c>
-      <c r="AX2" t="inlineStr">
+      <c r="BB2" t="inlineStr">
         <is>
           <t>true</t>
         </is>
       </c>
-      <c r="AY2" t="inlineStr">
+      <c r="BC2" t="inlineStr">
         <is>
           <t>22.50</t>
         </is>
       </c>
-      <c r="AZ2" t="inlineStr">
+      <c r="BD2" t="inlineStr">
         <is>
           <t>22.50</t>
         </is>
       </c>
-      <c r="BA2" t="inlineStr">
+      <c r="BE2" t="inlineStr">
         <is>
           <t>22.50</t>
         </is>
       </c>
-      <c r="BB2" t="inlineStr">
+      <c r="BF2" t="inlineStr">
         <is>
           <t>22.50</t>
         </is>
       </c>
-      <c r="BC2" t="inlineStr">
+      <c r="BG2" t="inlineStr">
         <is>
           <t>22.50</t>
         </is>
       </c>
-      <c r="BD2" t="inlineStr">
+      <c r="BH2" t="inlineStr">
         <is>
           <t>22.50</t>
         </is>
       </c>
-      <c r="BE2" t="inlineStr">
+      <c r="BI2" t="inlineStr">
         <is>
           <t>22.50</t>
         </is>
       </c>
-      <c r="BF2" t="inlineStr">
+      <c r="BJ2" t="inlineStr">
         <is>
           <t>22.50</t>
         </is>
       </c>
-      <c r="BG2" t="inlineStr">
+      <c r="BK2" t="inlineStr">
         <is>
           <t>22.50</t>
         </is>
       </c>
-      <c r="BH2" t="inlineStr">
+      <c r="BL2" t="inlineStr">
         <is>
           <t>22.50</t>
         </is>
       </c>
-      <c r="BI2" t="inlineStr">
+      <c r="BM2" t="inlineStr">
         <is>
           <t>22.50</t>
         </is>
       </c>
-      <c r="BJ2" t="inlineStr">
+      <c r="BN2" t="inlineStr">
         <is>
           <t>22.50</t>
         </is>
       </c>
-      <c r="BK2" t="inlineStr">
+      <c r="BO2" t="inlineStr">
         <is>
           <t>22.50</t>
         </is>
       </c>
-      <c r="BL2" t="inlineStr">
+      <c r="BP2" t="inlineStr">
         <is>
           <t>22.50</t>
         </is>
       </c>
-      <c r="BM2" t="inlineStr">
+      <c r="BQ2" t="inlineStr">
         <is>
           <t>22.50</t>
         </is>
       </c>
-      <c r="BN2" t="inlineStr">
+      <c r="BR2" t="inlineStr">
         <is>
           <t>22.50</t>
         </is>
       </c>
-      <c r="BO2" t="inlineStr">
+      <c r="BS2" t="inlineStr">
         <is>
           <t>22.50</t>
         </is>
       </c>
-      <c r="BP2" t="inlineStr">
+      <c r="BT2" t="inlineStr">
         <is>
           <t>22.50</t>
         </is>
       </c>
-      <c r="BQ2" t="inlineStr">
+      <c r="BU2" t="inlineStr">
         <is>
           <t>22.50</t>
         </is>
       </c>
-      <c r="BR2" t="inlineStr">
+      <c r="BV2" t="inlineStr">
         <is>
           <t>22.50</t>
         </is>
       </c>
-      <c r="BS2" t="inlineStr">
+      <c r="BW2" t="inlineStr">
         <is>
           <t>22.50</t>
         </is>
       </c>
-      <c r="BT2" t="inlineStr">
+      <c r="BX2" t="inlineStr">
         <is>
           <t>22.50</t>
         </is>
       </c>
-      <c r="BU2" t="inlineStr">
+      <c r="BY2" t="inlineStr">
         <is>
           <t>22.50</t>
         </is>
       </c>
-      <c r="BV2" t="inlineStr">
+      <c r="BZ2" t="inlineStr">
         <is>
           <t>22.50</t>
         </is>
       </c>
-      <c r="BW2" t="inlineStr">
+      <c r="CA2" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="BX2" t="inlineStr">
-        <is>
-          <t>3.610</t>
-        </is>
-      </c>
-      <c r="BY2" t="inlineStr">
-        <is>
-          <t>3.610</t>
-        </is>
-      </c>
-      <c r="BZ2" t="inlineStr">
+      <c r="CB2" t="inlineStr">
+        <is>
+          <t>3.610</t>
+        </is>
+      </c>
+      <c r="CC2" t="inlineStr">
+        <is>
+          <t>3.610</t>
+        </is>
+      </c>
+      <c r="CD2" t="inlineStr">
         <is>
           <t>3.611</t>
         </is>
       </c>
-      <c r="CA2" t="inlineStr">
-        <is>
-          <t>3.610</t>
-        </is>
-      </c>
-      <c r="CB2" t="inlineStr">
+      <c r="CE2" t="inlineStr">
+        <is>
+          <t>3.610</t>
+        </is>
+      </c>
+      <c r="CF2" t="inlineStr">
         <is>
           <t>3.611</t>
         </is>
       </c>
-      <c r="CC2" t="inlineStr">
-        <is>
-          <t>3.610</t>
-        </is>
-      </c>
-      <c r="CD2" t="inlineStr">
-        <is>
-          <t>3.610</t>
-        </is>
-      </c>
-      <c r="CE2" t="inlineStr">
-        <is>
-          <t>3.610</t>
-        </is>
-      </c>
-      <c r="CF2" t="inlineStr">
-        <is>
-          <t>3.610</t>
-        </is>
-      </c>
       <c r="CG2" t="inlineStr">
         <is>
           <t>3.610</t>
@@ -1782,39 +1802,39 @@
       </c>
       <c r="CH2" t="inlineStr">
         <is>
+          <t>3.610</t>
+        </is>
+      </c>
+      <c r="CI2" t="inlineStr">
+        <is>
+          <t>3.610</t>
+        </is>
+      </c>
+      <c r="CJ2" t="inlineStr">
+        <is>
+          <t>3.610</t>
+        </is>
+      </c>
+      <c r="CK2" t="inlineStr">
+        <is>
+          <t>3.610</t>
+        </is>
+      </c>
+      <c r="CL2" t="inlineStr">
+        <is>
           <t>3.611</t>
         </is>
       </c>
-      <c r="CI2" t="inlineStr">
+      <c r="CM2" t="inlineStr">
         <is>
           <t>3.611</t>
         </is>
       </c>
-      <c r="CJ2" t="inlineStr">
+      <c r="CN2" t="inlineStr">
         <is>
           <t>3.611</t>
         </is>
       </c>
-      <c r="CK2" t="inlineStr">
-        <is>
-          <t>3.610</t>
-        </is>
-      </c>
-      <c r="CL2" t="inlineStr">
-        <is>
-          <t>3.610</t>
-        </is>
-      </c>
-      <c r="CM2" t="inlineStr">
-        <is>
-          <t>3.610</t>
-        </is>
-      </c>
-      <c r="CN2" t="inlineStr">
-        <is>
-          <t>3.610</t>
-        </is>
-      </c>
       <c r="CO2" t="inlineStr">
         <is>
           <t>3.610</t>
@@ -1837,39 +1857,39 @@
       </c>
       <c r="CS2" t="inlineStr">
         <is>
+          <t>3.610</t>
+        </is>
+      </c>
+      <c r="CT2" t="inlineStr">
+        <is>
+          <t>3.610</t>
+        </is>
+      </c>
+      <c r="CU2" t="inlineStr">
+        <is>
+          <t>3.610</t>
+        </is>
+      </c>
+      <c r="CV2" t="inlineStr">
+        <is>
+          <t>3.610</t>
+        </is>
+      </c>
+      <c r="CW2" t="inlineStr">
+        <is>
           <t>3.609</t>
         </is>
       </c>
-      <c r="CT2" t="inlineStr">
-        <is>
-          <t>3.610</t>
-        </is>
-      </c>
-      <c r="CU2" t="inlineStr">
+      <c r="CX2" t="inlineStr">
+        <is>
+          <t>3.610</t>
+        </is>
+      </c>
+      <c r="CY2" t="inlineStr">
         <is>
           <t>3.609</t>
         </is>
       </c>
-      <c r="CV2" t="inlineStr">
-        <is>
-          <t>3.610</t>
-        </is>
-      </c>
-      <c r="CW2" t="inlineStr">
-        <is>
-          <t>3.610</t>
-        </is>
-      </c>
-      <c r="CX2" t="inlineStr">
-        <is>
-          <t>3.610</t>
-        </is>
-      </c>
-      <c r="CY2" t="inlineStr">
-        <is>
-          <t>3.610</t>
-        </is>
-      </c>
       <c r="CZ2" t="inlineStr">
         <is>
           <t>3.610</t>
@@ -1912,375 +1932,395 @@
       </c>
       <c r="DH2" t="inlineStr">
         <is>
+          <t>3.610</t>
+        </is>
+      </c>
+      <c r="DI2" t="inlineStr">
+        <is>
+          <t>3.610</t>
+        </is>
+      </c>
+      <c r="DJ2" t="inlineStr">
+        <is>
+          <t>3.610</t>
+        </is>
+      </c>
+      <c r="DK2" t="inlineStr">
+        <is>
+          <t>3.610</t>
+        </is>
+      </c>
+      <c r="DL2" t="inlineStr">
+        <is>
           <t>3.611</t>
         </is>
       </c>
-      <c r="DI2" t="inlineStr">
-        <is>
-          <t>3.610</t>
-        </is>
-      </c>
-      <c r="DJ2" t="inlineStr">
-        <is>
-          <t>3.610</t>
-        </is>
-      </c>
-      <c r="DK2" t="inlineStr">
+      <c r="DM2" t="inlineStr">
+        <is>
+          <t>3.610</t>
+        </is>
+      </c>
+      <c r="DN2" t="inlineStr">
+        <is>
+          <t>3.610</t>
+        </is>
+      </c>
+      <c r="DO2" t="inlineStr">
         <is>
           <t>3.609</t>
         </is>
       </c>
-      <c r="DL2" t="inlineStr">
+      <c r="DP2" t="inlineStr">
         <is>
           <t>3.611</t>
         </is>
       </c>
-      <c r="DM2" t="inlineStr">
+      <c r="DQ2" t="inlineStr">
         <is>
           <t>3.611</t>
         </is>
       </c>
-      <c r="DN2" t="inlineStr">
-        <is>
-          <t>3.610</t>
-        </is>
-      </c>
-      <c r="DO2" t="inlineStr">
-        <is>
-          <t>3.610</t>
-        </is>
-      </c>
-      <c r="DP2" t="inlineStr">
+      <c r="DR2" t="inlineStr">
+        <is>
+          <t>3.610</t>
+        </is>
+      </c>
+      <c r="DS2" t="inlineStr">
+        <is>
+          <t>3.610</t>
+        </is>
+      </c>
+      <c r="DT2" t="inlineStr">
         <is>
           <t>3.611</t>
         </is>
       </c>
-      <c r="DQ2" t="inlineStr">
-        <is>
-          <t>3.610</t>
-        </is>
-      </c>
-      <c r="DR2" t="inlineStr">
-        <is>
-          <t>3.610</t>
-        </is>
-      </c>
-      <c r="DS2" t="inlineStr">
+      <c r="DU2" t="inlineStr">
+        <is>
+          <t>3.610</t>
+        </is>
+      </c>
+      <c r="DV2" t="inlineStr">
+        <is>
+          <t>3.610</t>
+        </is>
+      </c>
+      <c r="DW2" t="inlineStr">
         <is>
           <t>3.609</t>
         </is>
       </c>
-      <c r="DT2" t="inlineStr">
-        <is>
-          <t>3.610</t>
-        </is>
-      </c>
-      <c r="DU2" t="inlineStr">
+      <c r="DX2" t="inlineStr">
+        <is>
+          <t>3.610</t>
+        </is>
+      </c>
+      <c r="DY2" t="inlineStr">
         <is>
           <t>3.611</t>
         </is>
       </c>
-      <c r="DV2" t="inlineStr">
-        <is>
-          <t>3.610</t>
-        </is>
-      </c>
-      <c r="DW2" t="inlineStr">
+      <c r="DZ2" t="inlineStr">
+        <is>
+          <t>3.610</t>
+        </is>
+      </c>
+      <c r="EA2" t="inlineStr">
         <is>
           <t>3.611</t>
         </is>
       </c>
-      <c r="DX2" t="inlineStr">
-        <is>
-          <t>3.610</t>
-        </is>
-      </c>
-      <c r="DY2" t="inlineStr">
-        <is>
-          <t>3.610</t>
-        </is>
-      </c>
-      <c r="DZ2" t="inlineStr">
-        <is>
-          <t>3.610</t>
-        </is>
-      </c>
-      <c r="EA2" t="inlineStr">
-        <is>
-          <t>3.610</t>
-        </is>
-      </c>
       <c r="EB2" t="inlineStr">
         <is>
+          <t>3.610</t>
+        </is>
+      </c>
+      <c r="EC2" t="inlineStr">
+        <is>
+          <t>3.610</t>
+        </is>
+      </c>
+      <c r="ED2" t="inlineStr">
+        <is>
+          <t>3.610</t>
+        </is>
+      </c>
+      <c r="EE2" t="inlineStr">
+        <is>
+          <t>3.610</t>
+        </is>
+      </c>
+      <c r="EF2" t="inlineStr">
+        <is>
           <t>3.609</t>
         </is>
       </c>
-      <c r="EC2" t="inlineStr">
+      <c r="EG2" t="inlineStr">
         <is>
           <t>3.609</t>
         </is>
       </c>
-      <c r="ED2" t="inlineStr">
-        <is>
-          <t>3.610</t>
-        </is>
-      </c>
-      <c r="EE2" t="inlineStr">
-        <is>
-          <t>3.610</t>
-        </is>
-      </c>
-      <c r="EF2" t="inlineStr">
+      <c r="EH2" t="inlineStr">
+        <is>
+          <t>3.610</t>
+        </is>
+      </c>
+      <c r="EI2" t="inlineStr">
+        <is>
+          <t>3.610</t>
+        </is>
+      </c>
+      <c r="EJ2" t="inlineStr">
         <is>
           <t>3.609</t>
         </is>
       </c>
-      <c r="EG2" t="inlineStr">
+      <c r="EK2" t="inlineStr">
         <is>
           <t>3.609</t>
         </is>
       </c>
-      <c r="EH2" t="inlineStr">
+      <c r="EL2" t="inlineStr">
         <is>
           <t>3.609</t>
         </is>
       </c>
-      <c r="EI2" t="inlineStr">
+      <c r="EM2" t="inlineStr">
         <is>
           <t>3.608</t>
         </is>
       </c>
-      <c r="EJ2" t="inlineStr">
-        <is>
-          <t>3.610</t>
-        </is>
-      </c>
-      <c r="EK2" t="inlineStr">
+      <c r="EN2" t="inlineStr">
+        <is>
+          <t>3.610</t>
+        </is>
+      </c>
+      <c r="EO2" t="inlineStr">
         <is>
           <t>3.611</t>
         </is>
       </c>
-      <c r="EL2" t="inlineStr">
-        <is>
-          <t>3.610</t>
-        </is>
-      </c>
-      <c r="EM2" t="inlineStr">
+      <c r="EP2" t="inlineStr">
+        <is>
+          <t>3.610</t>
+        </is>
+      </c>
+      <c r="EQ2" t="inlineStr">
         <is>
           <t>3.611</t>
         </is>
       </c>
-      <c r="EN2" t="inlineStr">
-        <is>
-          <t>3.610</t>
-        </is>
-      </c>
-      <c r="EO2" t="inlineStr">
-        <is>
-          <t>3.610</t>
-        </is>
-      </c>
-      <c r="EP2" t="inlineStr">
+      <c r="ER2" t="inlineStr">
+        <is>
+          <t>3.610</t>
+        </is>
+      </c>
+      <c r="ES2" t="inlineStr">
+        <is>
+          <t>3.610</t>
+        </is>
+      </c>
+      <c r="ET2" t="inlineStr">
         <is>
           <t>3.609</t>
         </is>
       </c>
-      <c r="EQ2" t="inlineStr">
+      <c r="EU2" t="inlineStr">
         <is>
           <t>3.609</t>
         </is>
       </c>
-      <c r="ER2" t="inlineStr">
+      <c r="EV2" t="inlineStr">
         <is>
           <t>3.609</t>
         </is>
       </c>
-      <c r="ES2" t="inlineStr">
+      <c r="EW2" t="inlineStr">
         <is>
           <t>3.609</t>
         </is>
       </c>
-      <c r="ET2" t="inlineStr">
+      <c r="EX2" t="inlineStr">
         <is>
           <t>3.609</t>
         </is>
       </c>
-      <c r="EU2" t="inlineStr">
-        <is>
-          <t>3.610</t>
-        </is>
-      </c>
-      <c r="EV2" t="inlineStr">
-        <is>
-          <t>3.610</t>
-        </is>
-      </c>
-      <c r="EW2" t="inlineStr">
+      <c r="EY2" t="inlineStr">
+        <is>
+          <t>3.610</t>
+        </is>
+      </c>
+      <c r="EZ2" t="inlineStr">
+        <is>
+          <t>3.610</t>
+        </is>
+      </c>
+      <c r="FA2" t="inlineStr">
         <is>
           <t>3.609</t>
         </is>
       </c>
-      <c r="EX2" t="inlineStr">
+      <c r="FB2" t="inlineStr">
         <is>
           <t>3.609</t>
         </is>
       </c>
-      <c r="EY2" t="inlineStr">
+      <c r="FC2" t="inlineStr">
         <is>
           <t>3.609</t>
         </is>
       </c>
-      <c r="EZ2" t="inlineStr">
-        <is>
-          <t>3.610</t>
-        </is>
-      </c>
-      <c r="FA2" t="inlineStr">
-        <is>
-          <t>3.610</t>
-        </is>
-      </c>
-      <c r="FB2" t="inlineStr">
-        <is>
-          <t>3.610</t>
-        </is>
-      </c>
-      <c r="FC2" t="inlineStr">
+      <c r="FD2" t="inlineStr">
+        <is>
+          <t>3.610</t>
+        </is>
+      </c>
+      <c r="FE2" t="inlineStr">
+        <is>
+          <t>3.610</t>
+        </is>
+      </c>
+      <c r="FF2" t="inlineStr">
+        <is>
+          <t>3.610</t>
+        </is>
+      </c>
+      <c r="FG2" t="inlineStr">
         <is>
           <t>3.611</t>
         </is>
       </c>
-      <c r="FD2" t="inlineStr">
+      <c r="FH2" t="inlineStr">
         <is>
           <t>3.611</t>
         </is>
       </c>
-      <c r="FE2" t="inlineStr">
-        <is>
-          <t>3.610</t>
-        </is>
-      </c>
-      <c r="FF2" t="inlineStr">
+      <c r="FI2" t="inlineStr">
+        <is>
+          <t>3.610</t>
+        </is>
+      </c>
+      <c r="FJ2" t="inlineStr">
         <is>
           <t>3.611</t>
         </is>
       </c>
-      <c r="FG2" t="inlineStr">
+      <c r="FK2" t="inlineStr">
         <is>
           <t>3.609</t>
         </is>
       </c>
-      <c r="FH2" t="inlineStr">
-        <is>
-          <t>3.610</t>
-        </is>
-      </c>
-      <c r="FI2" t="inlineStr">
+      <c r="FL2" t="inlineStr">
+        <is>
+          <t>3.610</t>
+        </is>
+      </c>
+      <c r="FM2" t="inlineStr">
         <is>
           <t>3.611</t>
         </is>
       </c>
-      <c r="FJ2" t="inlineStr">
+      <c r="FN2" t="inlineStr">
         <is>
           <t>3.611</t>
         </is>
       </c>
-      <c r="FK2" t="inlineStr">
-        <is>
-          <t>3.610</t>
-        </is>
-      </c>
-      <c r="FL2" t="inlineStr">
+      <c r="FO2" t="inlineStr">
+        <is>
+          <t>3.610</t>
+        </is>
+      </c>
+      <c r="FP2" t="inlineStr">
         <is>
           <t>3.611</t>
         </is>
       </c>
-      <c r="FM2" t="inlineStr">
-        <is>
-          <t>3.610</t>
-        </is>
-      </c>
-      <c r="FN2" t="inlineStr">
+      <c r="FQ2" t="inlineStr">
+        <is>
+          <t>3.610</t>
+        </is>
+      </c>
+      <c r="FR2" t="inlineStr">
         <is>
           <t>3.611</t>
         </is>
       </c>
-      <c r="FO2" t="inlineStr">
+      <c r="FS2" t="inlineStr">
         <is>
           <t>3.609</t>
         </is>
       </c>
-      <c r="FP2" t="inlineStr">
+      <c r="FT2" t="inlineStr">
         <is>
           <t>3.0</t>
         </is>
       </c>
-      <c r="FQ2" t="inlineStr">
+      <c r="FU2" t="inlineStr">
         <is>
           <t>42487</t>
         </is>
       </c>
-      <c r="FR2" t="inlineStr">
+      <c r="FV2" t="inlineStr">
         <is>
           <t>13697024</t>
         </is>
       </c>
-      <c r="FS2" t="inlineStr">
+      <c r="FW2" t="inlineStr">
         <is>
           <t>13828096</t>
         </is>
       </c>
-      <c r="FT2" t="inlineStr">
+      <c r="FX2" t="inlineStr">
         <is>
           <t>15361024</t>
         </is>
       </c>
-      <c r="FU2" t="inlineStr">
+      <c r="FY2" t="inlineStr">
         <is>
           <t>3.608</t>
         </is>
       </c>
-      <c r="FV2" t="inlineStr">
+      <c r="FZ2" t="inlineStr">
         <is>
           <t>3.611</t>
         </is>
       </c>
-      <c r="FW2" t="inlineStr">
+      <c r="GA2" t="inlineStr">
         <is>
           <t>22.500</t>
         </is>
       </c>
-      <c r="FX2" t="inlineStr">
+      <c r="GB2" t="inlineStr">
         <is>
           <t>3.611</t>
         </is>
       </c>
-      <c r="FY2" t="inlineStr">
+      <c r="GC2" t="inlineStr">
         <is>
           <t>"IO"</t>
         </is>
       </c>
-      <c r="FZ2" t="inlineStr">
+      <c r="GD2" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="GA2" t="inlineStr">
+      <c r="GE2" t="inlineStr">
         <is>
           <t>2.00000</t>
         </is>
       </c>
-      <c r="GB2" t="inlineStr">
+      <c r="GF2" t="inlineStr">
         <is>
           <t>4.00000</t>
         </is>
       </c>
-      <c r="GC2" t="inlineStr">
+      <c r="GG2" t="inlineStr">
         <is>
           <t>3.00891</t>
         </is>
       </c>
-      <c r="GD2" t="inlineStr">
+      <c r="GH2" t="inlineStr">
         <is>
           <t>"IO"</t>
         </is>

</xml_diff>